<commit_message>
Control measures of leaf disease been added
</commit_message>
<xml_diff>
--- a/disease.xlsx
+++ b/disease.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Leaf_Fastapi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4587AFD-01AE-4564-A18D-B4AF125956B0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8FE6480-EA68-4D51-970F-137568C010CD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{8F5F9B90-9E02-40F5-8D6B-4540B888C7AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,49 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
-  <si>
-    <t>50% yield reduction in severe cases .</t>
-  </si>
-  <si>
-    <t>The infection of the seed causes failure of seed germination, seedling mortality and reduces the grain quality and weight.</t>
-  </si>
-  <si>
-    <t>Dark brown or black spots also appear on glumes.</t>
-  </si>
-  <si>
-    <t>The seedlings die and affected nurseries can be often recognized from a distance by their brownish scorched appearance.</t>
-  </si>
-  <si>
-    <t>Lesions on the neck are grayish brown and causes the girdling of the neck and the panicle to fall over</t>
-  </si>
-  <si>
-    <t>The cut portion can be observed against the light to see the bacterial ooze streaming out from the cut ends into the water.</t>
-  </si>
-  <si>
-    <t>Seeds also infected (black or brown spots on glumes spots are covered by olivaceous velvety growth)</t>
-  </si>
-  <si>
-    <t>Internodal infection also occurs at the base of the plant which causes white panicles similar to that induced by yellow stem borer or water deficit</t>
-  </si>
-  <si>
-    <t>Yellowish bacterial ooze may be seen coming out of the cut ends.</t>
-  </si>
-  <si>
-    <t>Tungro virus disease affects all growth stages of the rice plant specifically the vegetative stage.</t>
-  </si>
-  <si>
-    <t>Infection also occurs on panicle, neck with brown colour appearance</t>
-  </si>
-  <si>
-    <t>To distinguish kresek symptoms from stem borer damage, the lower end of the infected seedling can be squeezed between the fingers.</t>
-  </si>
-  <si>
-    <t>Most panicles sterile or partially filled grains</t>
-  </si>
-  <si>
-    <t>Then several spots coalesce and the leaf dries up.</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>older lesions elliptical or spindle-shaped and whitish to gray with necrotic borders Several spots coalesce to  form big irregular patches.</t>
   </si>
@@ -75,9 +33,6 @@
     <t>Appearance of bacterial ooze that looks like a milky or opaque dewdrop on young lesions early in the morning</t>
   </si>
   <si>
-    <t>Delayed flowering, - panicles small and not completely exerted</t>
-  </si>
-  <si>
     <t>Spots measures 0.5 to 2.0mm in breadth - coalesce to form large patches.</t>
   </si>
   <si>
@@ -90,15 +45,9 @@
     <t>Discoloration begins from leaf tip and extends down to the blade or the lower leaf portion</t>
   </si>
   <si>
-    <t>initial symptoms are white to gray-green lesions or spots with brown borders</t>
-  </si>
-  <si>
     <t>Water-soaked to yellowish stripes on leaf blades or starting at leaf tips with a wavy margin</t>
   </si>
   <si>
-    <t>Control Measures: The main control measures are the use of disease-free or treated seeds and crop rotation. Stubble and straw should be burned after paddy harvesting on unhealthy soil. After seeing the disease, an additional 20 kg of potash fertilizer per acre should be applied to the water. Spraying chelated zinc at the rate of 1 gram per liter of water reduces the severity of the disease.</t>
-  </si>
-  <si>
     <t>Plants affected by tungro exhibit stunting and reduced tillering. Their leaves become yellow or orange-yellow, may also have rust-colored spots.</t>
   </si>
   <si>
@@ -117,9 +66,6 @@
     <t>Blast_control_measures</t>
   </si>
   <si>
-    <t>BB_control_measures</t>
-  </si>
-  <si>
     <t>Tungro</t>
   </si>
   <si>
@@ -139,6 +85,159 @@
   </si>
   <si>
     <t>Blast symptoms can occur on leaves, leaf collars, nodes and panicles. Leaf spots are typically elliptical (football shaped), with gray-white centers and brown to red-brown margins (Figure 1). Fully developed leaf lesions are approximately 0.4 to 0.7 inch long and 0.1 to 0.2 inch wide</t>
+  </si>
+  <si>
+    <t>Water-soaked, dark green or brown spots appear on the leaves, turning into yellow or brown necrotic lesions as the disease progresses.</t>
+  </si>
+  <si>
+    <t>Lesions may coalesce to form large patches on leaves, which may eventually lead to leaf death and defoliation.</t>
+  </si>
+  <si>
+    <t>Younger leaves may show a characteristic "kneading" or "wrinkling" appearance, where the leaf blade and leaf sheath are tightly folded along the midrib.</t>
+  </si>
+  <si>
+    <t>In severe cases, the stems and leaf sheaths of the infected plants may also show symptoms of dark green or brown water-soaked spots.</t>
+  </si>
+  <si>
+    <t>The infected plants may become stunted and their yield may be reduced.</t>
+  </si>
+  <si>
+    <t>The disease may spread rapidly under favorable conditions such as high humidity, warm temperatures, and heavy rainfall.</t>
+  </si>
+  <si>
+    <t>white to gray-green lesions or spots with brown borders</t>
+  </si>
+  <si>
+    <t>Leaf lesions: Blast disease causes small, grayish or whitish lesions on the leaves of the rice plant. The lesions can be oval or elongated in shape, and they may have a reddish-brown border. As the disease progresses, the lesions may enlarge and merge together, causing larger areas of damage on the leaves.</t>
+  </si>
+  <si>
+    <t>Neck blast: Neck blast is a more severe form of blast disease that affects the stem and panicle of the rice plant. This can cause the stem to wither and die, which can result in significant yield losses. Neck blast is characterized by dark, sunken lesions that appear on the stem of the rice plant, just below the panicle.</t>
+  </si>
+  <si>
+    <t>Collar rot: Collar rot is another severe form of blast disease that affects the base of the rice plant. This can cause the plant to wilt and die, and can result in complete crop failure. Collar rot is characterized by a dark, sunken lesion at the base of the rice plant, near the soil line.</t>
+  </si>
+  <si>
+    <t>Blasting: The name "blast disease" comes from the characteristic "blasting" symptom that occurs when the panicle is infected. Blasting refers to the premature drying and death of the panicle, which can result in significant yield losses. The panicle may turn gray or white in color, and the grains may be partially or completely empty.</t>
+  </si>
+  <si>
+    <t>Leaf Spots: Small, oval to circular spots with brown centers and yellowish-brown margins appear on leaves. These spots can merge, and cause the leaves to turn yellow and dry out.</t>
+  </si>
+  <si>
+    <t>Lesions on Sheath: The lesions may also appear on the sheath of the rice plant. They are usually brown with a yellowish margin. The sheath may become brown and dry, and cause the stem to break easily.</t>
+  </si>
+  <si>
+    <t>Stem Rot: Brown spots may appear on the stem near the water line. The infected part of the stem becomes brown, and may rot, causing the plant to fall over.</t>
+  </si>
+  <si>
+    <t>Panicle Infection: In severe cases, the fungus can infect the rice panicle. The infected grains are discolored and have small brown spots. They become shriveled and do not fill completely, which reduces the yield.</t>
+  </si>
+  <si>
+    <t>General Weakness: As the disease progresses, the rice plant becomes weak and stunted, and may not produce a good harvest.</t>
+  </si>
+  <si>
+    <t>Yellowing of leaves: Infected plants may show yellowing or chlorosis of leaves, which starts at the tips and margins and spreads towards the base of the leaf.</t>
+  </si>
+  <si>
+    <t>Stunted growth: Plants infected with tungro virus may show stunted growth, which can result in a reduced yield.</t>
+  </si>
+  <si>
+    <t>Necrosis of leaves: Infected leaves may show necrosis or death of tissues, resulting in the formation of yellow or brown spots or streaks on the leaves.</t>
+  </si>
+  <si>
+    <t>Reduced tillering: Infected plants may show reduced tillering or the formation of fewer tillers.</t>
+  </si>
+  <si>
+    <t>Delayed maturity: Infected plants may take longer to mature, resulting in delayed harvest.</t>
+  </si>
+  <si>
+    <t>Reduced yield: Tungro rice disease can significantly reduce rice yield, resulting in economic losses for farmers.</t>
+  </si>
+  <si>
+    <t>Use resistant varieties: Plant resistant rice varieties that are less susceptible to bacterial blight. There are several rice varieties available that have been bred for resistance to bacterial blight.</t>
+  </si>
+  <si>
+    <t>Crop rotation: Rotate rice crops with non-host crops such as wheat, maize, or soybeans to reduce the build-up of the bacterial blight pathogen in the soil.</t>
+  </si>
+  <si>
+    <t>Sanitation: Remove and destroy infected plants and plant debris from the field to prevent the spread of the disease to healthy plants. Clean and disinfect tools and equipment before and after use.</t>
+  </si>
+  <si>
+    <t>Seed treatment: Treat seeds with fungicides or antibiotics to kill the bacterial blight pathogen before planting.</t>
+  </si>
+  <si>
+    <t>Use of biocontrol agents: Apply biocontrol agents such as Bacillus subtilis and Pseudomonas fluorescens to the soil or plant surfaces to suppress the growth of the bacterial blight pathogen.</t>
+  </si>
+  <si>
+    <t>Avoid overhead irrigation: Bacterial blight spreads through water, so avoid overhead irrigation and instead use drip or furrow irrigation to reduce the spread of the disease.</t>
+  </si>
+  <si>
+    <t>Use of copper-based fungicides: Apply copper-based fungicides such as copper sulfate to control bacterial blight in rice plants. However, be careful not to exceed the recommended doses as it can cause phytotoxicity.</t>
+  </si>
+  <si>
+    <t>Use resistant varieties: Plant resistant varieties of rice that are less susceptible to blast disease. This is the most effective and economic way to manage the disease.</t>
+  </si>
+  <si>
+    <t>Crop rotation: Rotate rice with other crops to reduce the inoculum of the fungus in the soil. This will help to break the disease cycle and prevent the build-up of the pathogen.</t>
+  </si>
+  <si>
+    <t>Seed treatment: Treat the seeds with a fungicide to reduce the risk of infection. This will help to protect the seedlings from the disease.</t>
+  </si>
+  <si>
+    <t>Timely planting: Plant rice at the recommended time to avoid late planting, which is a major risk factor for blast disease.</t>
+  </si>
+  <si>
+    <t>Sanitation: Remove and destroy crop residues, which may harbor the pathogen, and weed the fields to prevent the spread of the disease.</t>
+  </si>
+  <si>
+    <t>Fungicides: Use fungicides to control the disease, but only as a last resort. Fungicides should be applied at the right time, in the right amount and in the right manner.</t>
+  </si>
+  <si>
+    <t>Water management: Manage the water levels in the rice fields to reduce the incidence and severity of blast disease. Proper water management can reduce the humidity and the amount of free water on the leaves, which are conducive to the growth of the fungus.</t>
+  </si>
+  <si>
+    <t>Plant resistant varieties: Planting resistant varieties is the most effective way to manage tungro disease. Several varieties with resistance to the disease are available, and farmers should choose those varieties.</t>
+  </si>
+  <si>
+    <t>Early planting: Early planting is recommended to avoid the peak population of the insect vector, which is the green leafhopper.</t>
+  </si>
+  <si>
+    <t>Sanitation: Farmers should remove infected plants and weed hosts from their fields to reduce the insect vector's population and slow down the spread of the disease.</t>
+  </si>
+  <si>
+    <t>Insecticide application: Insecticides can be used to control the insect vector of the disease, but farmers should follow the recommended application rate and timing to avoid resistance development.</t>
+  </si>
+  <si>
+    <t>Crop rotation: Crop rotation with non-rice crops can reduce the insect vector population and break the disease cycle.</t>
+  </si>
+  <si>
+    <t>Monitoring: Farmers should regularly monitor their rice fields for symptoms of the disease and insect populations. Early detection can help in controlling the disease and minimizing yield losses.</t>
+  </si>
+  <si>
+    <t>Community effort: Since tungro disease is transmitted by insects, it can easily spread from one field to another. Farmers in the community should work together to control the disease by coordinating their efforts and following the same control measures.</t>
+  </si>
+  <si>
+    <t>Crop rotation: Brown spot disease can survive in rice straw, so it is important to rotate crops to avoid planting rice in the same field year after year. Planting other crops like soybeans, corn, or wheat can break the disease cycle.</t>
+  </si>
+  <si>
+    <t>Use resistant varieties: Planting resistant varieties of rice is an effective way to prevent brown spot disease. Many new varieties of rice have been developed that are resistant to brown spot, so farmers should choose resistant varieties when possible.</t>
+  </si>
+  <si>
+    <t>Good water management: Brown spot disease thrives in humid conditions, so farmers should avoid over-watering and make sure there is good drainage in the fields.</t>
+  </si>
+  <si>
+    <t>Proper fertilization: Over-fertilization can lead to an increase in the severity of brown spot disease. Farmers should apply the right amount of fertilizer based on soil testing to avoid over-fertilizing.</t>
+  </si>
+  <si>
+    <t>Timely application of fungicides: If brown spot disease is detected early, it can be controlled by applying fungicides. Farmers should consult with their local agriculture extension office to determine the right fungicides to use and the appropriate timing for application.</t>
+  </si>
+  <si>
+    <t>Good field sanitation: Farmers should remove diseased plant debris from the field and burn it to prevent the spread of the disease to healthy plants.</t>
+  </si>
+  <si>
+    <t>Use of biological control: Farmers can use biological control agents such as Trichoderma, Pseudomonas fluorescens, and Bacillus subtilis, which have been found to be effective against brown spot disease.</t>
+  </si>
+  <si>
+    <t>Bacterialblight_control_measures</t>
   </si>
 </sst>
 </file>
@@ -523,209 +622,297 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C36ABC5E-C0AF-47F7-9D13-7D1DCFCCC686}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.5703125" customWidth="1"/>
-    <col min="2" max="2" width="52.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="3" width="23.28515625" customWidth="1"/>
     <col min="4" max="4" width="17.5703125" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" customWidth="1"/>
     <col min="6" max="6" width="24.140625" customWidth="1"/>
-    <col min="7" max="8" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
+    <col min="8" max="8" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="4" spans="1:8" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
+        <v>37</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>11</v>
+      <c r="A6" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="7" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
+        <v>32</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="108" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>4</v>
+      <c r="A8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="9" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="C9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="1"/>
+        <v>33</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+    <row r="10" spans="1:8" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2" t="s">
-        <v>0</v>
-      </c>
+    <row r="11" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>